<commit_message>
fixes to account assistant
working on updater
</commit_message>
<xml_diff>
--- a/Order_Database.xlsx
+++ b/Order_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\big\TH_for_Distribution_Accounting_assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1509CBB9-7F6D-4490-BEB5-A513A40B639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFB8B7E-7E58-42EC-AF05-FDA118A504CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,9 +405,6 @@
     <t>علبة هدايا Y9 Prime 2019</t>
   </si>
   <si>
-    <t>Samsung EG /  A 13 4/128</t>
-  </si>
-  <si>
     <t>WearFit Pro/X8+ Ultra</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>777</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Samsung EG /  A 13 4/128</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -496,11 +496,22 @@
       <right style="thick">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top style="thick">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
+      <bottom style="hair">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,11 +522,11 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color rgb="FFD3D3D3"/>
+      <top style="hair">
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
+      <bottom style="hair">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,8 +537,8 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color rgb="FFD3D3D3"/>
+      <top style="hair">
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -540,56 +551,39 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FFD3D3D3"/>
+      <bottom style="hair">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thick">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thick">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -597,24 +591,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,729 +1003,729 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="66.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-    </row>
-    <row r="2" spans="1:1" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-    </row>
-    <row r="3" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+    </row>
+    <row r="2" spans="1:1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="86" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
     <row r="87" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="104" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="9" t="s">
-        <v>129</v>
+    <row r="105" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+    <row r="108" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="9" t="s">
-        <v>129</v>
+    <row r="109" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="7" t="s">
+      <c r="A110" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="7" t="s">
-        <v>129</v>
+      <c r="A111" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="6" t="s">
-        <v>129</v>
+      <c r="A117" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
+    <row r="119" spans="1:1" s="8" customFormat="1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="7" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="A128" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="A129" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="A131" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="A132" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="A133" s="5" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="A134" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="A135" s="5" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="A136" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="A137" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="A138" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="A139" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="24" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>